<commit_message>
aggiunto la revised edition della relazione del reticolo
</commit_message>
<xml_diff>
--- a/Prisma/Data%20Analysis/reticolo prisma.xlsx
+++ b/Prisma/Data%20Analysis/reticolo prisma.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaco\OneDrive\Dokumente\backup surface\2-anno\laboratorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\passa\Documents\Scuola\Corsi\Fisica\Laboratorio\LaboratorioOtticaElettronicaFModerna\Git\Reticolo-prisma\Prisma\Data%20Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="19590" windowHeight="10058" tabRatio="479" activeTab="1"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="19590" windowHeight="10065" tabRatio="479"/>
   </bookViews>
   <sheets>
     <sheet name="dati raccolti" sheetId="1" r:id="rId1"/>
@@ -284,12 +284,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="20% - Colore 5" xfId="3" builtinId="46"/>
-    <cellStyle name="40% - Colore 5" xfId="4" builtinId="47"/>
-    <cellStyle name="60% - Colore 5" xfId="5" builtinId="48"/>
-    <cellStyle name="Cella da controllare" xfId="1" builtinId="23"/>
-    <cellStyle name="Colore 5" xfId="2" builtinId="45"/>
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="20% - Accent5" xfId="3" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="4" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="5" builtinId="48"/>
+    <cellStyle name="Accent5" xfId="2" builtinId="45"/>
+    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -305,7 +305,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -603,26 +603,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q149"/>
   <sheetViews>
-    <sheetView topLeftCell="A122" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q143" sqref="Q143"/>
+    <sheetView tabSelected="1" topLeftCell="E25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A117" sqref="A117:B122"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.796875" customWidth="1"/>
-    <col min="4" max="4" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:17" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
@@ -645,7 +645,7 @@
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -692,7 +692,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <f>354</f>
         <v>354</v>
@@ -749,7 +749,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>35</v>
       </c>
@@ -804,7 +804,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>30</v>
       </c>
@@ -859,7 +859,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>25</v>
       </c>
@@ -914,7 +914,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>25</v>
       </c>
@@ -970,7 +970,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>30</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>16</v>
       </c>
@@ -1034,7 +1034,7 @@
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>0</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>1.0467612188835984</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <f>INT(DEGREES(D16))</f>
         <v>59</v>
@@ -1125,7 +1125,7 @@
         <v>0.24933275028463492</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <f t="shared" ref="A17:A22" si="9">INT(DEGREES(D17))</f>
         <v>59</v>
@@ -1175,7 +1175,7 @@
         <v>0.74799825085390481</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <f t="shared" si="9"/>
         <v>59</v>
@@ -1225,7 +1225,7 @@
         <v>1.4959965017062868</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <f t="shared" si="9"/>
         <v>59</v>
@@ -1275,7 +1275,7 @@
         <v>0.74799825085390481</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <f t="shared" si="9"/>
         <v>59</v>
@@ -1325,7 +1325,7 @@
         <v>0.74799825085390481</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <f t="shared" si="9"/>
         <v>59</v>
@@ -1375,7 +1375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <f t="shared" si="9"/>
         <v>59</v>
@@ -1397,8 +1397,8 @@
         <v>3.0042805007150824E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="24" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>11</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>0</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D26">
         <v>178</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>2.9166666666666669E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D27">
         <v>358</v>
       </c>
@@ -1462,12 +1462,12 @@
         <v>2.9166666666666669E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <f>0.00000040463</f>
         <v>4.0462999999999999E-7</v>
@@ -1485,7 +1485,7 @@
         <v>3.9499999999999998E-10</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>-1.2108871480675114</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>104</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>7.41761319630177E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>104</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>104</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>252</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>252</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>252</v>
       </c>
@@ -1784,7 +1784,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K40">
         <f>AVERAGE(K34:K39)</f>
         <v>1.2984756944444447</v>
@@ -1794,12 +1794,12 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43">
         <f>0.0000004078</f>
         <v>4.0779999999999999E-7</v>
@@ -1816,7 +1816,7 @@
         <v>3.0099999999999999E-10</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>19</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>0</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>-1.2066368630130377</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>104</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>7.398402930146326E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>104</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>104</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>252</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="13">
         <v>252</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>252</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K53">
         <f>AVERAGE(K47:K52)</f>
         <v>1.293152777777778</v>
@@ -2125,12 +2125,12 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>12</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57">
         <f>0.00000043583</f>
         <v>4.3583000000000001E-7</v>
@@ -2147,7 +2147,7 @@
         <v>5.0100000000000003E-10</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>19</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>0</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>-1.1765487567409849</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>106</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>7.2637710492251604E-4</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>106</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>106</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>250</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="13">
         <v>250</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>250</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K67">
         <f>AVERAGE(K61:K66)</f>
         <v>1.2557708333333333</v>
@@ -2456,12 +2456,12 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>12</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71">
         <f>0.00000049228</f>
         <v>4.9228000000000001E-7</v>
@@ -2478,7 +2478,7 @@
         <v>5.0000000000000003E-10</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>19</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>0</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>-1.1368493906397061</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>109</v>
       </c>
@@ -2582,7 +2582,7 @@
         <v>7.0898690751389334E-4</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>109</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>109</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>247</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>247</v>
       </c>
@@ -2738,7 +2738,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>247</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K81">
         <f>AVERAGE(K75:K80)</f>
         <v>1.2072083333333334</v>
@@ -2787,12 +2787,12 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>12</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85">
         <f>0.00000049698</f>
         <v>4.9698000000000005E-7</v>
@@ -2809,7 +2809,7 @@
         <v>2.7399999999999998E-10</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>19</v>
       </c>
@@ -2820,7 +2820,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>0</v>
       </c>
@@ -2866,7 +2866,7 @@
         <v>-1.1368493906397061</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>109</v>
       </c>
@@ -2913,7 +2913,7 @@
         <v>7.0898690751389334E-4</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>109</v>
       </c>
@@ -2952,7 +2952,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>109</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>247</v>
       </c>
@@ -3030,7 +3030,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>247</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>247</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K95">
         <f>AVERAGE(K89:K94)</f>
         <v>1.2072083333333334</v>
@@ -3118,12 +3118,12 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>12</v>
       </c>
@@ -3131,7 +3131,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99">
         <f>0.00000054604</f>
         <v>5.4603999999999998E-7</v>
@@ -3140,7 +3140,7 @@
         <v>3E-10</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>19</v>
       </c>
@@ -3151,7 +3151,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>0</v>
       </c>
@@ -3197,7 +3197,7 @@
         <v>-1.1122976971467435</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>111</v>
       </c>
@@ -3244,7 +3244,7 @@
         <v>6.984520273395962E-4</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>111</v>
       </c>
@@ -3283,7 +3283,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>111</v>
       </c>
@@ -3322,7 +3322,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>245</v>
       </c>
@@ -3361,7 +3361,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>246</v>
       </c>
@@ -3400,7 +3400,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>246</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K109">
         <f>AVERAGE(K103:K108)</f>
         <v>1.1775798611111112</v>
@@ -3449,12 +3449,12 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>12</v>
       </c>
@@ -3462,7 +3462,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113">
         <f>0.00000057694</f>
         <v>5.7693999999999998E-7</v>
@@ -3471,7 +3471,7 @@
         <v>2.99E-10</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>19</v>
       </c>
@@ -3482,7 +3482,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>0</v>
       </c>
@@ -3528,7 +3528,7 @@
         <v>-1.10183117257709</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>112</v>
       </c>
@@ -3575,7 +3575,7 @@
         <v>6.9401347006651788E-4</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>112</v>
       </c>
@@ -3614,7 +3614,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>112</v>
       </c>
@@ -3653,7 +3653,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>245</v>
       </c>
@@ -3692,7 +3692,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>245</v>
       </c>
@@ -3731,7 +3731,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>245</v>
       </c>
@@ -3770,7 +3770,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K123">
         <f>AVERAGE(K117:K122)</f>
         <v>1.1650381944444448</v>
@@ -3780,12 +3780,12 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>12</v>
       </c>
@@ -3793,7 +3793,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A126">
         <f>0.00000057901</f>
         <v>5.7901000000000005E-7</v>
@@ -3802,7 +3802,7 @@
         <v>8.2800000000000004E-10</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>19</v>
       </c>
@@ -3813,7 +3813,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>0</v>
       </c>
@@ -3859,7 +3859,7 @@
         <v>-1.1009366675942949</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>112</v>
       </c>
@@ -3906,7 +3906,7 @@
         <v>6.9363561198346668E-4</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>112</v>
       </c>
@@ -3945,7 +3945,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>112</v>
       </c>
@@ -3984,7 +3984,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>245</v>
       </c>
@@ -4023,7 +4023,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>245</v>
       </c>
@@ -4062,7 +4062,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>245</v>
       </c>
@@ -4101,7 +4101,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K136">
         <f>AVERAGE(K130:K135)</f>
         <v>1.16396875</v>
@@ -4111,12 +4111,12 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>12</v>
       </c>
@@ -4124,7 +4124,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A139">
         <f>0.00000062334</f>
         <v>6.2333999999999997E-7</v>
@@ -4133,7 +4133,7 @@
         <v>5.1499999999999998E-10</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>19</v>
       </c>
@@ -4144,7 +4144,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>0</v>
       </c>
@@ -4190,7 +4190,7 @@
         <v>-1.0751271152768147</v>
       </c>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>113</v>
       </c>
@@ -4237,7 +4237,7 @@
         <v>6.8283467461972738E-4</v>
       </c>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>113</v>
       </c>
@@ -4276,7 +4276,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>113</v>
       </c>
@@ -4315,7 +4315,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>243</v>
       </c>
@@ -4354,7 +4354,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>243</v>
       </c>
@@ -4393,7 +4393,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>243</v>
       </c>
@@ -4432,7 +4432,7 @@
         <v>5.8333333333333338E-4</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K149">
         <f>AVERAGE(K143:K148)</f>
         <v>1.1332708333333334</v>
@@ -4452,26 +4452,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -4488,7 +4488,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>1/'dati raccolti'!A30^2</f>
         <v>6107786419350.2119</v>
@@ -4510,7 +4510,7 @@
         <v>5.0483306043599191E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>1/'dati raccolti'!A43^2</f>
         <v>6013198730685.9072</v>
@@ -4532,7 +4532,7 @@
         <v>5.0239466483190023E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>1/'dati raccolti'!A57^2</f>
         <v>5264604583138.6875</v>
@@ -4554,7 +4554,7 @@
         <v>4.8529463595261635E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>1/'dati raccolti'!A71^2</f>
         <v>4126440774030.7617</v>
@@ -4576,7 +4576,7 @@
         <v>4.6319175896293325E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>1/'dati raccolti'!A85^2</f>
         <v>4048761331594.2637</v>
@@ -4598,7 +4598,7 @@
         <v>4.6319175896274061E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <f>1/'dati raccolti'!A99^2</f>
         <v>3353907525771.9224</v>
@@ -4620,7 +4620,7 @@
         <v>4.4694309469421331E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>1/'dati raccolti'!A113^2</f>
         <v>3004268191458.873</v>
@@ -4642,7 +4642,7 @@
         <v>4.4416092188621281E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>1/'dati raccolti'!A126^2</f>
         <v>2982825664463.8418</v>
@@ -4664,7 +4664,7 @@
         <v>4.4368077167162411E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <f>1/'dati raccolti'!A139^2</f>
         <v>2573653089799.3716</v>
@@ -4686,13 +4686,13 @@
         <v>4.2995897387832988E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F13">
         <f>SLOPE(B4:B12,A4:A12)</f>
         <v>6.7475496238438128E-14</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14">
         <f>PEARSON(B4:B12,A4:A12)</f>
         <v>0.99705166013887114</v>
@@ -4702,25 +4702,25 @@
         <v>2.9899682465287998</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D18" s="12"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>40</v>
       </c>

</xml_diff>